<commit_message>
A lot of changes, left off at cov/corr matrix and started doing the min_vol matrix markowitz. Other important changes, created a new folder in equities, called "retired", where I put some securities which had too many nan values. That folder is excluded from the main database but didn't want to delete it "just in case".
</commit_message>
<xml_diff>
--- a/portfolio-optimization/data/raw/alternatives/aim_data_centr_etf.xlsx
+++ b/portfolio-optimization/data/raw/alternatives/aim_data_centr_etf.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{960D789A-E49E-4745-96FF-7CAC780DD358}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBEA2F47-90F8-4FDB-A316-6952B8105610}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -54,6 +54,9 @@
     <t>Ticker</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Digital Realty Trust Inc</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
   </si>
   <si>
     <t>DLR</t>
+  </si>
+  <si>
+    <t>Digital Reality Trust, Inc. owns, acquires, repositions, and manages technology-related real estate. The portfolio is located throughout the US and in England.</t>
   </si>
 </sst>
 </file>
@@ -433,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1272"/>
+  <dimension ref="A1:H1272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +469,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>45813</v>
       </c>
@@ -478,16 +487,19 @@
         <v>1543776</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>45812</v>
       </c>
@@ -501,7 +513,7 @@
         <v>1637834</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>45811</v>
       </c>
@@ -515,7 +527,7 @@
         <v>1667937</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>45810</v>
       </c>
@@ -529,7 +541,7 @@
         <v>1705781</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>45807</v>
       </c>
@@ -543,7 +555,7 @@
         <v>1709689</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>45806</v>
       </c>
@@ -557,7 +569,7 @@
         <v>1546257</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>45805</v>
       </c>
@@ -571,7 +583,7 @@
         <v>1533727</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>45804</v>
       </c>
@@ -585,7 +597,7 @@
         <v>1517822</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>45800</v>
       </c>
@@ -599,7 +611,7 @@
         <v>1494549</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>45799</v>
       </c>
@@ -613,7 +625,7 @@
         <v>1518488</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>45798</v>
       </c>
@@ -627,7 +639,7 @@
         <v>1577086</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>45797</v>
       </c>
@@ -641,7 +653,7 @@
         <v>1637995</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>45796</v>
       </c>
@@ -655,7 +667,7 @@
         <v>1684071</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>45793</v>
       </c>
@@ -669,7 +681,7 @@
         <v>1760832</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>45792</v>
       </c>

</xml_diff>